<commit_message>
Add last iteration result
</commit_message>
<xml_diff>
--- a/EvaluationIterations.xlsx
+++ b/EvaluationIterations.xlsx
@@ -5,23 +5,27 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Dropbox\Intech-Spi\Semestres\2015-2\S3\Projets\The Lawbreaker Jellyfishes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Bureau\Git-Stuff\Project-TLJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="15600" windowHeight="8010" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="15600" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="It0" sheetId="1" r:id="rId1"/>
     <sheet name="It1" sheetId="6" r:id="rId2"/>
-    <sheet name="Constantes" sheetId="4" state="hidden" r:id="rId3"/>
+    <sheet name="It2" sheetId="7" r:id="rId3"/>
+    <sheet name="Constantes" sheetId="4" state="hidden" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162912"/>
+  <externalReferences>
+    <externalReference r:id="rId5"/>
+  </externalReferences>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="67">
   <si>
     <t>The Lawbreaker Jellyfishes - It0</t>
   </si>
@@ -171,13 +175,64 @@
   </si>
   <si>
     <t>Echelle</t>
+  </si>
+  <si>
+    <t>Vous avez tous les atouts pour être plus convainquant</t>
+  </si>
+  <si>
+    <t>Jérome encore un effort</t>
+  </si>
+  <si>
+    <t>Manque de dynamisme</t>
+  </si>
+  <si>
+    <t>Soyez plus explicites !</t>
+  </si>
+  <si>
+    <t>Trop de branches et ce avec un nommage discutable</t>
+  </si>
+  <si>
+    <t>Un seul test, et sans assert…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pas encore de graphismes + visiblement quelques bugs </t>
+  </si>
+  <si>
+    <t>Dommage pour le plantage</t>
+  </si>
+  <si>
+    <t>Gestion des évènements et des combats</t>
+  </si>
+  <si>
+    <t>Système de résurrection</t>
+  </si>
+  <si>
+    <t>Système de notification</t>
+  </si>
+  <si>
+    <t>Système de sauvegarde</t>
+  </si>
+  <si>
+    <t>Interaction morgue</t>
+  </si>
+  <si>
+    <t>Pas encore de graphismes dignes de ce nom</t>
+  </si>
+  <si>
+    <t>Interaction milice</t>
+  </si>
+  <si>
+    <t>Commentaires</t>
+  </si>
+  <si>
+    <t>The Lawbreaker Jellyfishes - It2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,7 +256,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -280,8 +335,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="38">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -752,6 +813,169 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -759,7 +983,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -978,6 +1202,30 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="10" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="11" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="10" fontId="0" fillId="8" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1047,30 +1295,85 @@
     <xf numFmtId="10" fontId="0" fillId="13" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="41" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="7" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="12" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="12" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="47" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="11" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="11" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="11" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="48" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="41" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="10" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="10" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="14" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="11" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="50" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1089,8 +1392,29 @@
 </styleSheet>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Feuil1"/>
+      <sheetName val="Constantes"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1">
+        <row r="1">
+          <cell r="B1">
+            <v>5</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1379,10 +1703,10 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
@@ -1390,7 +1714,7 @@
     <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.5" thickBot="1">
+    <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="69" t="s">
         <v>0</v>
       </c>
@@ -1406,7 +1730,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="93" t="s">
         <v>4</v>
       </c>
@@ -1428,7 +1752,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="94"/>
       <c r="B3" s="79"/>
       <c r="C3" s="18" t="s">
@@ -1445,7 +1769,7 @@
         <v>3.2000000000000001E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="94"/>
       <c r="B4" s="79"/>
       <c r="C4" s="18" t="s">
@@ -1463,7 +1787,7 @@
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="94"/>
       <c r="B5" s="79"/>
       <c r="C5" s="18" t="s">
@@ -1480,7 +1804,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1">
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="95"/>
       <c r="B6" s="80"/>
       <c r="C6" s="19" t="s">
@@ -1497,7 +1821,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="96" t="s">
         <v>10</v>
       </c>
@@ -1519,7 +1843,7 @@
         <v>3.2000000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="97"/>
       <c r="B8" s="82"/>
       <c r="C8" s="18" t="s">
@@ -1536,7 +1860,7 @@
         <v>3.2000000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="97"/>
       <c r="B9" s="82"/>
       <c r="C9" s="18" t="s">
@@ -1554,7 +1878,7 @@
       </c>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="97"/>
       <c r="B10" s="82"/>
       <c r="C10" s="18" t="s">
@@ -1571,7 +1895,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1">
+    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="98"/>
       <c r="B11" s="83"/>
       <c r="C11" s="19" t="s">
@@ -1588,7 +1912,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="99" t="s">
         <v>16</v>
       </c>
@@ -1610,7 +1934,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="100"/>
       <c r="B13" s="85"/>
       <c r="C13" s="18" t="s">
@@ -1627,7 +1951,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="100"/>
       <c r="B14" s="85"/>
       <c r="C14" s="21" t="s">
@@ -1645,7 +1969,7 @@
       </c>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="100"/>
       <c r="B15" s="85"/>
       <c r="C15" s="18" t="s">
@@ -1663,7 +1987,7 @@
       </c>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1">
+    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="101"/>
       <c r="B16" s="86"/>
       <c r="C16" s="19" t="s">
@@ -1680,7 +2004,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="72" t="s">
         <v>22</v>
       </c>
@@ -1702,7 +2026,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="73"/>
       <c r="B18" s="88"/>
       <c r="C18" s="21" t="s">
@@ -1719,7 +2043,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="73"/>
       <c r="B19" s="88"/>
       <c r="C19" s="24" t="s">
@@ -1736,7 +2060,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1">
+    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="74"/>
       <c r="B20" s="89"/>
       <c r="C20" s="23" t="s">
@@ -1753,7 +2077,7 @@
         <v>6.4000000000000001E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="75" t="s">
         <v>27</v>
       </c>
@@ -1775,7 +2099,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="76"/>
       <c r="B22" s="91"/>
       <c r="C22" s="30" t="s">
@@ -1792,7 +2116,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1">
+    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="77"/>
       <c r="B23" s="92"/>
       <c r="C23" s="31" t="s">
@@ -1809,7 +2133,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="63" t="s">
         <v>31</v>
       </c>
@@ -1831,7 +2155,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="64"/>
       <c r="B25" s="67"/>
       <c r="C25" s="27" t="s">
@@ -1848,7 +2172,7 @@
         <v>4.0000000000000008E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" thickBot="1">
+    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="65"/>
       <c r="B26" s="68"/>
       <c r="C26" s="28" t="s">
@@ -1865,7 +2189,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75" thickBot="1">
+    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D27" s="1"/>
       <c r="E27" s="2" t="s">
         <v>35</v>
@@ -1875,7 +2199,7 @@
         <v>0.79000000000000026</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
     </row>
@@ -1907,11 +2231,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="19.85546875" customWidth="1"/>
     <col min="3" max="3" width="35.42578125" bestFit="1" customWidth="1"/>
@@ -1920,7 +2244,7 @@
     <col min="6" max="6" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5" thickBot="1">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="69" t="s">
         <v>36</v>
       </c>
@@ -1936,11 +2260,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="125" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="127">
+      <c r="B2" s="104">
         <f>SUM(D2:D5)/D28</f>
         <v>0.13333333333333333</v>
       </c>
@@ -1958,9 +2282,9 @@
         <v>1.1111111111111112E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="126"/>
-      <c r="B3" s="128"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="103"/>
+      <c r="B3" s="105"/>
       <c r="C3" s="30" t="s">
         <v>39</v>
       </c>
@@ -1975,9 +2299,9 @@
         <v>1.1111111111111112E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="126"/>
-      <c r="B4" s="128"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="103"/>
+      <c r="B4" s="105"/>
       <c r="C4" s="30" t="s">
         <v>40</v>
       </c>
@@ -1992,9 +2316,9 @@
         <v>8.8888888888888892E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A5" s="126"/>
-      <c r="B5" s="128"/>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="103"/>
+      <c r="B5" s="105"/>
       <c r="C5" s="30" t="s">
         <v>41</v>
       </c>
@@ -2009,11 +2333,11 @@
         <v>2.2222222222222223E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="129" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="106" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="131">
+      <c r="B6" s="108">
         <f>SUM(D6:D9)/D28</f>
         <v>0.13333333333333333</v>
       </c>
@@ -2031,9 +2355,9 @@
         <v>1.1111111111111112E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="130"/>
-      <c r="B7" s="132"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="107"/>
+      <c r="B7" s="109"/>
       <c r="C7" s="30" t="s">
         <v>39</v>
       </c>
@@ -2048,9 +2372,9 @@
         <v>1.1111111111111112E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="130"/>
-      <c r="B8" s="132"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="107"/>
+      <c r="B8" s="109"/>
       <c r="C8" s="30" t="s">
         <v>40</v>
       </c>
@@ -2065,9 +2389,9 @@
         <v>8.8888888888888892E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A9" s="130"/>
-      <c r="B9" s="132"/>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="107"/>
+      <c r="B9" s="109"/>
       <c r="C9" s="54" t="s">
         <v>41</v>
       </c>
@@ -2082,11 +2406,11 @@
         <v>2.2222222222222223E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="105" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="113" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="108">
+      <c r="B10" s="116">
         <f>SUM(D10:D13)/D28</f>
         <v>0.13333333333333333</v>
       </c>
@@ -2104,9 +2428,9 @@
         <v>1.1111111111111112E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="106"/>
-      <c r="B11" s="109"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="114"/>
+      <c r="B11" s="117"/>
       <c r="C11" s="30" t="s">
         <v>39</v>
       </c>
@@ -2121,9 +2445,9 @@
         <v>1.1111111111111112E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="106"/>
-      <c r="B12" s="109"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="114"/>
+      <c r="B12" s="117"/>
       <c r="C12" s="30" t="s">
         <v>40</v>
       </c>
@@ -2138,9 +2462,9 @@
         <v>8.8888888888888892E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A13" s="107"/>
-      <c r="B13" s="110"/>
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="115"/>
+      <c r="B13" s="118"/>
       <c r="C13" s="54" t="s">
         <v>41</v>
       </c>
@@ -2155,11 +2479,11 @@
         <v>2.2222222222222223E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="111" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="114">
+      <c r="B14" s="122">
         <f>SUM(D14:D17)/D28</f>
         <v>0.13333333333333333</v>
       </c>
@@ -2177,9 +2501,9 @@
         <v>1.1111111111111112E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="112"/>
-      <c r="B15" s="115"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="120"/>
+      <c r="B15" s="123"/>
       <c r="C15" s="30" t="s">
         <v>39</v>
       </c>
@@ -2194,9 +2518,9 @@
         <v>1.1111111111111112E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="112"/>
-      <c r="B16" s="115"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="120"/>
+      <c r="B16" s="123"/>
       <c r="C16" s="30" t="s">
         <v>40</v>
       </c>
@@ -2211,9 +2535,9 @@
         <v>8.8888888888888892E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A17" s="113"/>
-      <c r="B17" s="116"/>
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="121"/>
+      <c r="B17" s="124"/>
       <c r="C17" s="54" t="s">
         <v>41</v>
       </c>
@@ -2228,11 +2552,11 @@
         <v>2.2222222222222223E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="119" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="127" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="122">
+      <c r="B18" s="130">
         <f>SUM(D18:D21)/D28</f>
         <v>0.13333333333333333</v>
       </c>
@@ -2250,9 +2574,9 @@
         <v>1.1111111111111112E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="120"/>
-      <c r="B19" s="123"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="128"/>
+      <c r="B19" s="131"/>
       <c r="C19" s="30" t="s">
         <v>39</v>
       </c>
@@ -2267,9 +2591,9 @@
         <v>1.1111111111111112E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="120"/>
-      <c r="B20" s="123"/>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="128"/>
+      <c r="B20" s="131"/>
       <c r="C20" s="30" t="s">
         <v>40</v>
       </c>
@@ -2284,9 +2608,9 @@
         <v>8.8888888888888892E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A21" s="121"/>
-      <c r="B21" s="124"/>
+    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="129"/>
+      <c r="B21" s="132"/>
       <c r="C21" s="31" t="s">
         <v>41</v>
       </c>
@@ -2301,11 +2625,11 @@
         <v>2.2222222222222223E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="117">
+      <c r="B22" s="125">
         <f>SUM(D22:D24)/D28</f>
         <v>0.16666666666666666</v>
       </c>
@@ -2323,9 +2647,9 @@
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="73"/>
-      <c r="B23" s="118"/>
+      <c r="B23" s="126"/>
       <c r="C23" s="44" t="s">
         <v>46</v>
       </c>
@@ -2340,9 +2664,9 @@
         <v>2.6666666666666665E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" thickBot="1">
+    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="73"/>
-      <c r="B24" s="118"/>
+      <c r="B24" s="126"/>
       <c r="C24" s="45" t="s">
         <v>26</v>
       </c>
@@ -2357,11 +2681,11 @@
         <v>6.0000000000000005E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="102">
+      <c r="B25" s="110">
         <f>SUM(D25:D27)/D28</f>
         <v>0.16666666666666666</v>
       </c>
@@ -2379,9 +2703,9 @@
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="76"/>
-      <c r="B26" s="103"/>
+      <c r="B26" s="111"/>
       <c r="C26" s="30" t="s">
         <v>29</v>
       </c>
@@ -2396,9 +2720,9 @@
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75" thickBot="1">
+    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="77"/>
-      <c r="B27" s="104"/>
+      <c r="B27" s="112"/>
       <c r="C27" s="31" t="s">
         <v>30</v>
       </c>
@@ -2413,7 +2737,7 @@
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" thickBot="1">
+    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="51" t="s">
         <v>47</v>
       </c>
@@ -2431,11 +2755,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
     <mergeCell ref="A25:A27"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="A10:A13"/>
@@ -2446,6 +2765,11 @@
     <mergeCell ref="B22:B24"/>
     <mergeCell ref="A18:A21"/>
     <mergeCell ref="B18:B21"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2456,15 +2780,692 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" customWidth="1"/>
+    <col min="7" max="7" width="50.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="69" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="169" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="168" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="167" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="166">
+        <f>SUM(D2:D5)/D32</f>
+        <v>7.3170731707317069E-2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="36">
+        <v>1</v>
+      </c>
+      <c r="E2" s="37">
+        <v>5</v>
+      </c>
+      <c r="F2" s="143">
+        <f>(D2*E2/[1]Constantes!$B$1)/D$32</f>
+        <v>1.2195121951219513E-2</v>
+      </c>
+      <c r="G2" s="165" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="164"/>
+      <c r="B3" s="163"/>
+      <c r="C3" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="38">
+        <v>1</v>
+      </c>
+      <c r="E3" s="39">
+        <v>5</v>
+      </c>
+      <c r="F3" s="138">
+        <f>(D3*E3/[1]Constantes!$B$1)/D$32</f>
+        <v>1.2195121951219513E-2</v>
+      </c>
+      <c r="G3" s="148"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="164"/>
+      <c r="B4" s="163"/>
+      <c r="C4" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="38">
+        <v>3</v>
+      </c>
+      <c r="E4" s="39">
+        <v>4</v>
+      </c>
+      <c r="F4" s="138">
+        <f>(D4*E4/[1]Constantes!$B$1)/D$32</f>
+        <v>2.9268292682926828E-2</v>
+      </c>
+      <c r="G4" s="148"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="164"/>
+      <c r="B5" s="163"/>
+      <c r="C5" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="40">
+        <v>1</v>
+      </c>
+      <c r="E5" s="41">
+        <v>5</v>
+      </c>
+      <c r="F5" s="136">
+        <f>(D5*E5/[1]Constantes!$B$1)/D$32</f>
+        <v>1.2195121951219513E-2</v>
+      </c>
+      <c r="G5" s="148"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="102" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="162">
+        <f>SUM(D6:D9)/D32</f>
+        <v>7.3170731707317069E-2</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="36">
+        <v>1</v>
+      </c>
+      <c r="E6" s="37">
+        <v>5</v>
+      </c>
+      <c r="F6" s="143">
+        <f>(D6*E6/[1]Constantes!$B$1)/D$32</f>
+        <v>1.2195121951219513E-2</v>
+      </c>
+      <c r="G6" s="148"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="103"/>
+      <c r="B7" s="160"/>
+      <c r="C7" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="38">
+        <v>1</v>
+      </c>
+      <c r="E7" s="39">
+        <v>5</v>
+      </c>
+      <c r="F7" s="138">
+        <f>(D7*E7/[1]Constantes!$B$1)/D$32</f>
+        <v>1.2195121951219513E-2</v>
+      </c>
+      <c r="G7" s="148"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="103"/>
+      <c r="B8" s="160"/>
+      <c r="C8" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="42">
+        <v>3</v>
+      </c>
+      <c r="E8" s="41">
+        <v>4</v>
+      </c>
+      <c r="F8" s="161">
+        <f>(D8*E8/[1]Constantes!$B$1)/D$32</f>
+        <v>2.9268292682926828E-2</v>
+      </c>
+      <c r="G8" s="148"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="103"/>
+      <c r="B9" s="160"/>
+      <c r="C9" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="55">
+        <v>1</v>
+      </c>
+      <c r="E9" s="56">
+        <v>5</v>
+      </c>
+      <c r="F9" s="159">
+        <f>(D9*E9/[1]Constantes!$B$1)/D$32</f>
+        <v>1.2195121951219513E-2</v>
+      </c>
+      <c r="G9" s="148"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="106" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="158">
+        <f>SUM(D10:D13)/D32</f>
+        <v>7.3170731707317069E-2</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="36">
+        <v>1</v>
+      </c>
+      <c r="E10" s="37">
+        <v>5</v>
+      </c>
+      <c r="F10" s="143">
+        <f>(D10*E10/[1]Constantes!$B$1)/D$32</f>
+        <v>1.2195121951219513E-2</v>
+      </c>
+      <c r="G10" s="148"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="107"/>
+      <c r="B11" s="157"/>
+      <c r="C11" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="38">
+        <v>1</v>
+      </c>
+      <c r="E11" s="39">
+        <v>5</v>
+      </c>
+      <c r="F11" s="138">
+        <f>(D11*E11/[1]Constantes!$B$1)/D$32</f>
+        <v>1.2195121951219513E-2</v>
+      </c>
+      <c r="G11" s="148"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="107"/>
+      <c r="B12" s="157"/>
+      <c r="C12" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="42">
+        <v>3</v>
+      </c>
+      <c r="E12" s="39">
+        <v>4</v>
+      </c>
+      <c r="F12" s="138">
+        <f>(D12*E12/[1]Constantes!$B$1)/D$32</f>
+        <v>2.9268292682926828E-2</v>
+      </c>
+      <c r="G12" s="148"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="156"/>
+      <c r="B13" s="155"/>
+      <c r="C13" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="55">
+        <v>1</v>
+      </c>
+      <c r="E13" s="58">
+        <v>5</v>
+      </c>
+      <c r="F13" s="154">
+        <f>(D13*E13/[1]Constantes!$B$1)/D$32</f>
+        <v>1.2195121951219513E-2</v>
+      </c>
+      <c r="G13" s="148"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="113" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="116">
+        <f>SUM(D14:D17)/D32</f>
+        <v>7.3170731707317069E-2</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="36">
+        <v>1</v>
+      </c>
+      <c r="E14" s="37">
+        <v>5</v>
+      </c>
+      <c r="F14" s="143">
+        <f>(D14*E14/[1]Constantes!$B$1)/D$32</f>
+        <v>1.2195121951219513E-2</v>
+      </c>
+      <c r="G14" s="148"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="114"/>
+      <c r="B15" s="117"/>
+      <c r="C15" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="38">
+        <v>1</v>
+      </c>
+      <c r="E15" s="39">
+        <v>5</v>
+      </c>
+      <c r="F15" s="138">
+        <f>(D15*E15/[1]Constantes!$B$1)/D$32</f>
+        <v>1.2195121951219513E-2</v>
+      </c>
+      <c r="G15" s="148"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="114"/>
+      <c r="B16" s="117"/>
+      <c r="C16" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="42">
+        <v>3</v>
+      </c>
+      <c r="E16" s="39">
+        <v>4</v>
+      </c>
+      <c r="F16" s="138">
+        <f>(D16*E16/[1]Constantes!$B$1)/D$32</f>
+        <v>2.9268292682926828E-2</v>
+      </c>
+      <c r="G16" s="148"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="115"/>
+      <c r="B17" s="118"/>
+      <c r="C17" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="55">
+        <v>1</v>
+      </c>
+      <c r="E17" s="60">
+        <v>5</v>
+      </c>
+      <c r="F17" s="153">
+        <f>(D17*E17/[1]Constantes!$B$1)/D$32</f>
+        <v>1.2195121951219513E-2</v>
+      </c>
+      <c r="G17" s="148"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="152" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="151">
+        <f>SUM(D18:D21)/D32</f>
+        <v>0.2073170731707317</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="36">
+        <v>1</v>
+      </c>
+      <c r="E18" s="37">
+        <v>5</v>
+      </c>
+      <c r="F18" s="143">
+        <f>(D18*E18/[1]Constantes!$B$1)/D$32</f>
+        <v>1.2195121951219513E-2</v>
+      </c>
+      <c r="G18" s="148"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="150"/>
+      <c r="B19" s="149"/>
+      <c r="C19" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="40">
+        <v>1</v>
+      </c>
+      <c r="E19" s="41">
+        <v>5</v>
+      </c>
+      <c r="F19" s="136">
+        <f>(D19*E19/[1]Constantes!$B$1)/D$32</f>
+        <v>1.2195121951219513E-2</v>
+      </c>
+      <c r="G19" s="148"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="150"/>
+      <c r="B20" s="149"/>
+      <c r="C20" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="40">
+        <v>12</v>
+      </c>
+      <c r="E20" s="41">
+        <v>4</v>
+      </c>
+      <c r="F20" s="136">
+        <f>(D20*E20/[1]Constantes!$B$1)/D$32</f>
+        <v>0.11707317073170731</v>
+      </c>
+      <c r="G20" s="148"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="147"/>
+      <c r="B21" s="146"/>
+      <c r="C21" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="46">
+        <v>3</v>
+      </c>
+      <c r="E21" s="47">
+        <v>5</v>
+      </c>
+      <c r="F21" s="134">
+        <f>(D21*E21/[1]Constantes!$B$1)/D$32</f>
+        <v>3.6585365853658534E-2</v>
+      </c>
+      <c r="G21" s="145"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="127" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="130">
+        <f>SUM(D22:D25)/D32</f>
+        <v>0.2073170731707317</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="36">
+        <v>1</v>
+      </c>
+      <c r="E22" s="37">
+        <v>5</v>
+      </c>
+      <c r="F22" s="143">
+        <f>(D22*E22/[1]Constantes!$B$1)/D$32</f>
+        <v>1.2195121951219513E-2</v>
+      </c>
+      <c r="G22" s="142"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="128"/>
+      <c r="B23" s="131"/>
+      <c r="C23" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="40">
+        <v>1</v>
+      </c>
+      <c r="E23" s="41">
+        <v>4</v>
+      </c>
+      <c r="F23" s="136">
+        <f>(D23*E23/[1]Constantes!$B$1)/D$32</f>
+        <v>9.7560975609756097E-3</v>
+      </c>
+      <c r="G23" s="135" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="128"/>
+      <c r="B24" s="131"/>
+      <c r="C24" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="40">
+        <v>12</v>
+      </c>
+      <c r="E24" s="41">
+        <v>4</v>
+      </c>
+      <c r="F24" s="136">
+        <f>(D24*E24/[1]Constantes!$B$1)/D$32</f>
+        <v>0.11707317073170731</v>
+      </c>
+      <c r="G24" s="135" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="129"/>
+      <c r="B25" s="132"/>
+      <c r="C25" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="46">
+        <v>3</v>
+      </c>
+      <c r="E25" s="47">
+        <v>3</v>
+      </c>
+      <c r="F25" s="134">
+        <f>(D25*E25/[1]Constantes!$B$1)/D$32</f>
+        <v>2.1951219512195124E-2</v>
+      </c>
+      <c r="G25" s="133" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="72" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="125">
+        <f>SUM(D26:D28)/D32</f>
+        <v>0.14634146341463414</v>
+      </c>
+      <c r="C26" s="144" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="36">
+        <v>3</v>
+      </c>
+      <c r="E26" s="37">
+        <v>5</v>
+      </c>
+      <c r="F26" s="143">
+        <f>(D26*E26/[1]Constantes!$B$1)/D$32</f>
+        <v>3.6585365853658534E-2</v>
+      </c>
+      <c r="G26" s="142"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="73"/>
+      <c r="B27" s="126"/>
+      <c r="C27" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="40">
+        <v>3</v>
+      </c>
+      <c r="E27" s="41">
+        <v>4</v>
+      </c>
+      <c r="F27" s="136">
+        <f>(D27*E27/[1]Constantes!$B$1)/D$32</f>
+        <v>2.9268292682926828E-2</v>
+      </c>
+      <c r="G27" s="135" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="74"/>
+      <c r="B28" s="141"/>
+      <c r="C28" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="46">
+        <v>6</v>
+      </c>
+      <c r="E28" s="47">
+        <v>4</v>
+      </c>
+      <c r="F28" s="134">
+        <f>(D28*E28/[1]Constantes!$B$1)/D$32</f>
+        <v>5.8536585365853655E-2</v>
+      </c>
+      <c r="G28" s="133" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="76" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="111">
+        <f>SUM(D29:D31)/D32</f>
+        <v>0.14634146341463414</v>
+      </c>
+      <c r="C29" s="140" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="139">
+        <v>4</v>
+      </c>
+      <c r="E29" s="39">
+        <v>4</v>
+      </c>
+      <c r="F29" s="138">
+        <f>(D29*E29/[1]Constantes!$B$1)/D$32</f>
+        <v>3.9024390243902439E-2</v>
+      </c>
+      <c r="G29" s="137" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="76"/>
+      <c r="B30" s="111"/>
+      <c r="C30" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="49">
+        <v>4</v>
+      </c>
+      <c r="E30" s="41">
+        <v>4</v>
+      </c>
+      <c r="F30" s="136">
+        <f>(D30*E30/[1]Constantes!$B$1)/D$32</f>
+        <v>3.9024390243902439E-2</v>
+      </c>
+      <c r="G30" s="135" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="77"/>
+      <c r="B31" s="112"/>
+      <c r="C31" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="50">
+        <v>4</v>
+      </c>
+      <c r="E31" s="47">
+        <v>4</v>
+      </c>
+      <c r="F31" s="134">
+        <f>(D31*E31/[1]Constantes!$B$1)/D$32</f>
+        <v>3.9024390243902439E-2</v>
+      </c>
+      <c r="G31" s="133" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32" s="52">
+        <f>SUM(D2:D31)</f>
+        <v>82</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F32" s="53">
+        <f>SUM(F2:F31)</f>
+        <v>0.84390243902439055</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="G2:G21"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="A26:A28"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>49</v>
       </c>

</xml_diff>